<commit_message>
Updated Demand Estimates on Data Validation File
Updated rightmost table on the "Demand Data" sheet of Data Validation and Analysis.xlsx
Updated Estimates for Demand for Industry,Commercial,Residential, and Transport.
Industry and Transport are found in Figure 19-5 of the below link, but the rest are not so likely second eyes needed:
https://www.apec.org/docs/default-source/publications/2022/9/apec-energy-demand-and-supply-outlook-8th-edition---volume-ii/222_ewg_apec-energy-demand-and-supply-outlook_vol-2_o.pdf?sfvrsn=ce82bc8a_2
</commit_message>
<xml_diff>
--- a/CustomThailandScenarios/Data/Data Validation and Analysis.xlsx
+++ b/CustomThailandScenarios/Data/Data Validation and Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mresb\Documents\Oxford\Small Group Exercise\MOD. Modelling\OSE. OSeMOSYS\ThailandEnergyModelling\CustomThailandScenarios\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/ThailandEnergyModelling/CustomThailandScenarios/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF65B031-F003-4616-A2D2-316081ED27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A0AEE7-342A-234A-9E87-CD92958C6C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19160" windowHeight="17600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Energy Consumption" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,28 @@
     <sheet name="Carbon Emissions" sheetId="4" r:id="rId7"/>
     <sheet name="Labour" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="89">
   <si>
     <t>Total</t>
   </si>
@@ -269,6 +280,36 @@
   </si>
   <si>
     <t>https://www.irena.org/-/media/Files/IRENA/Agency/Statistics/Statistical_Profiles/Asia/Thailand_Asia_RE_SP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.apec.org/docs/default-source/publications/2022/9/apec-energy-demand-and-supply-outlook-8th-edition---volume-ii/222_ewg_apec-energy-demand-and-supply-outlook_vol-2_o.pdf?sfvrsn=ce82bc8a_2</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 19-5. Energy demand by sector in REF, 2000-2050 (PJ) </t>
+  </si>
+  <si>
+    <t>2050 Projection</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>Actual Projection found or estimated?</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>Estimated!</t>
+  </si>
+  <si>
+    <t>2050 Per component</t>
+  </si>
+  <si>
+    <t>2050 Total</t>
   </si>
 </sst>
 </file>
@@ -276,9 +317,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +357,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="AvenirLTStd"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -348,14 +395,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -363,10 +410,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,9 +431,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +471,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -529,7 +577,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -671,7 +719,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,13 +733,13 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:10">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -705,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:10">
       <c r="D4">
         <v>2019</v>
       </c>
@@ -716,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:10">
       <c r="D5">
         <v>2022</v>
       </c>
@@ -727,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:10">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -738,14 +786,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:10">
       <c r="H9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:10">
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -761,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:10">
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -777,7 +825,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:10">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -789,7 +837,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:10">
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
@@ -803,7 +851,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:10">
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
@@ -819,7 +867,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:10">
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
@@ -831,7 +879,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:10">
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
@@ -843,7 +891,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10">
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
@@ -853,7 +901,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10">
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
@@ -867,7 +915,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10">
       <c r="C21" s="2" t="s">
         <v>0</v>
       </c>
@@ -889,18 +937,18 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:11">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:11">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -911,7 +959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:11">
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -927,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:11">
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
@@ -943,7 +991,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:11">
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
@@ -957,7 +1005,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:11">
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
@@ -971,7 +1019,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:11">
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
@@ -990,7 +1038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:11">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +1050,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:11">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1062,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:11">
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1026,14 +1074,14 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:11">
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:11">
       <c r="E16" s="1">
         <f>SUM(E7:E14)</f>
         <v>100</v>
@@ -1046,19 +1094,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEB0D8E-EAFC-4C3E-829E-14F472141A8B}">
-  <dimension ref="B4:Z26"/>
+  <dimension ref="B3:AB26"/>
   <sheetViews>
-    <sheetView zoomScale="52" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="94" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.81640625" customWidth="1"/>
-    <col min="3" max="3" width="23.36328125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:28">
+      <c r="AA3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28">
       <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
@@ -1071,8 +1127,22 @@
       <c r="R4" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="AB4" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28">
+      <c r="X5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28">
       <c r="B6" s="5" t="s">
         <v>34</v>
       </c>
@@ -1083,7 +1153,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:28">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>31</v>
@@ -1106,8 +1176,14 @@
       <c r="V7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W7" t="s">
+        <v>87</v>
+      </c>
+      <c r="X7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1160,8 +1236,22 @@
         <f>100*U8/(U$8+U$11+U$14+U$17)</f>
         <v>12.249710602217075</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W8">
+        <f>T8*(1+Y8)</f>
+        <v>259.4583494998891</v>
+      </c>
+      <c r="X8">
+        <f>U8*(1+Y8)</f>
+        <v>627.96650000000011</v>
+      </c>
+      <c r="Y8">
+        <v>0.75</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1195,8 +1285,12 @@
       </c>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W9">
+        <f>T9*(1+$Y8)</f>
+        <v>257.95570533661027</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1231,8 +1325,12 @@
       </c>
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W10">
+        <f>T10*(1+$Y8)</f>
+        <v>110.55244516350074</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1285,8 +1383,25 @@
         <f>100*U11/(U$8+U$11+U$14+U$17)</f>
         <v>45.934998066129822</v>
       </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W11">
+        <f>T11*(1+Y11)</f>
+        <v>987.36642289287136</v>
+      </c>
+      <c r="X11">
+        <v>2304</v>
+      </c>
+      <c r="Y11">
+        <f>(X11-U11)/U11</f>
+        <v>0.71224605213581127</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="J12" t="s">
@@ -1306,8 +1421,12 @@
       </c>
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W12">
+        <f>T12*(1+Y11)</f>
+        <v>658.24428198027772</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1333,8 +1452,12 @@
       </c>
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W13">
+        <f>T13*(1+Y11)</f>
+        <v>658.38929512685104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28">
       <c r="I14" t="s">
         <v>8</v>
       </c>
@@ -1372,8 +1495,25 @@
         <f>100*U14/(U$8+U$11+U$14+U$17)</f>
         <v>35.55740351387454</v>
       </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W14">
+        <f>T14*(1+Y14)</f>
+        <v>391.99999997050423</v>
+      </c>
+      <c r="X14">
+        <v>1960</v>
+      </c>
+      <c r="Y14">
+        <f>(X14-U14)/U14</f>
+        <v>0.88171320386634411</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28">
       <c r="J15" t="s">
         <v>48</v>
       </c>
@@ -1390,8 +1530,12 @@
       </c>
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="W15">
+        <f>T15*(1+Y14)</f>
+        <v>842.79999997345385</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28">
       <c r="J16" t="s">
         <v>49</v>
       </c>
@@ -1408,8 +1552,12 @@
       </c>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
-    </row>
-    <row r="17" spans="9:26" x14ac:dyDescent="0.35">
+      <c r="W16">
+        <f>T16*(1+Y14)</f>
+        <v>725.20000005604197</v>
+      </c>
+    </row>
+    <row r="17" spans="9:27">
       <c r="I17" t="s">
         <v>12</v>
       </c>
@@ -1445,8 +1593,22 @@
         <f>100*U17/(U$8+U$11+U$14+U$17)</f>
         <v>6.2578878177785642</v>
       </c>
-    </row>
-    <row r="18" spans="9:26" x14ac:dyDescent="0.35">
+      <c r="W17">
+        <f>T17*(1+Y17)</f>
+        <v>53.303491415542425</v>
+      </c>
+      <c r="X17">
+        <f>U17*(1+Y17)</f>
+        <v>320.80299999999994</v>
+      </c>
+      <c r="Y17">
+        <v>0.75</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="9:27">
       <c r="J18" t="s">
         <v>51</v>
       </c>
@@ -1463,8 +1625,12 @@
       </c>
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
-    </row>
-    <row r="20" spans="9:26" x14ac:dyDescent="0.35">
+      <c r="W18">
+        <f>T18*(1+Y17)</f>
+        <v>267.49950858445754</v>
+      </c>
+    </row>
+    <row r="20" spans="9:27">
       <c r="K20" s="5">
         <f>SUM(K8:K18)</f>
         <v>3590.1801382100007</v>
@@ -1474,17 +1640,17 @@
         <v>2929.3590000000008</v>
       </c>
     </row>
-    <row r="23" spans="9:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="9:27">
       <c r="T23">
         <v>30.459137951738501</v>
       </c>
     </row>
-    <row r="24" spans="9:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="9:27">
       <c r="T24">
         <v>152.85686204826146</v>
       </c>
     </row>
-    <row r="26" spans="9:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="9:27">
       <c r="T26">
         <v>447.88971998589267</v>
       </c>
@@ -1503,7 +1669,7 @@
       <c r="Y26">
         <v>447.88971998589267</v>
       </c>
-      <c r="Z26">
+      <c r="AA26">
         <v>447.88971998589267</v>
       </c>
     </row>
@@ -1520,17 +1686,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7319DC5-69BF-455D-B06E-60BC43ACC689}">
   <dimension ref="A2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1538,7 +1704,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="B4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1552,12 +1718,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="K5" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="I6" t="s">
         <v>18</v>
       </c>
@@ -1568,7 +1734,7 @@
         <v>4.468</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="I7" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1745,7 @@
         <v>20.804200000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="I8" t="s">
         <v>70</v>
       </c>
@@ -1590,7 +1756,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="J9" s="7" t="s">
         <v>58</v>
       </c>
@@ -1598,7 +1764,7 @@
         <v>42.88</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="I10" t="s">
         <v>73</v>
       </c>
@@ -1609,7 +1775,7 @@
         <v>3.6389999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="J11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1617,7 +1783,7 @@
         <v>0.14799999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="I12" t="s">
         <v>72</v>
       </c>
@@ -1628,7 +1794,7 @@
         <v>27.132000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="I13" t="s">
         <v>19</v>
       </c>
@@ -1639,7 +1805,7 @@
         <v>3.0649999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="J14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1647,7 +1813,7 @@
         <v>42.88</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="J15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1821,7 @@
         <v>0.13850000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="J16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1663,7 +1829,7 @@
         <v>4.4695</v>
       </c>
     </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:11">
       <c r="I17" t="s">
         <v>71</v>
       </c>
@@ -1687,14 +1853,14 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4">
       <c r="C5" t="s">
         <v>39</v>
       </c>
@@ -1702,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1710,11 +1876,11 @@
         <v>35176</v>
       </c>
       <c r="D6">
-        <f>100*C6/SUM(C$6:C$12)</f>
+        <f t="shared" ref="D6:D12" si="0">100*C6/SUM(C$6:C$12)</f>
         <v>19.914287493560238</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -1722,11 +1888,11 @@
         <v>657</v>
       </c>
       <c r="D7">
-        <f>100*C7/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>0.37194925185550026</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1734,11 +1900,11 @@
         <v>110052</v>
       </c>
       <c r="D8">
-        <f>100*C8/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>62.304047283411741</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1746,11 +1912,11 @@
         <v>4682</v>
       </c>
       <c r="D9">
-        <f>100*C9/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.6506337856734432</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -1758,11 +1924,11 @@
         <v>17503</v>
       </c>
       <c r="D10">
-        <f>100*C10/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>9.9090224584883124</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -1770,11 +1936,11 @@
         <v>5015</v>
       </c>
       <c r="D11">
-        <f>100*C11/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.8391560092166421</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1782,7 +1948,7 @@
         <v>3552</v>
       </c>
       <c r="D12">
-        <f>100*C12/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.01090371779412</v>
       </c>
     </row>
@@ -1799,9 +1965,9 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:7">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7">
       <c r="D5" t="s">
         <v>6</v>
       </c>
@@ -1826,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:7">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -1847,18 +2013,18 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:5">
       <c r="C3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:5">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1867,7 +2033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:5">
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1876,7 +2042,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:5">
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1885,7 +2051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:5">
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1894,29 +2060,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:5">
       <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:5">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:5">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:5">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:5">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -1924,7 +2090,7 @@
         <v>372648</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:5">
       <c r="D13" t="s">
         <v>28</v>
       </c>
@@ -1942,12 +2108,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:5">
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -1955,12 +2121,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:5">
       <c r="C4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:5">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -1968,7 +2134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:5">
       <c r="C6" t="s">
         <v>30</v>
       </c>
@@ -1982,6 +2148,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D2C1BEFAF870748BACCC527472C8EB2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487ae15c868a429603055564894ba096">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1041d1a3-2b21-46e0-8139-4e1099981477" xmlns:ns3="66da9736-248e-4959-a705-07c73b004417" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="194ea4c5e0e7bff924a75701159686b7" ns2:_="" ns3:_="">
     <xsd:import namespace="1041d1a3-2b21-46e0-8139-4e1099981477"/>
@@ -2158,15 +2333,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2174,6 +2340,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415282BC-98EB-4742-A7DA-4D7B8E81DDAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3650B4B3-630C-4862-A6F7-7FA0C9B693D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2188,14 +2362,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415282BC-98EB-4742-A7DA-4D7B8E81DDAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated Capacity and Generation for 2021
</commit_message>
<xml_diff>
--- a/CustomThailandScenarios/Data/Data Validation and Analysis.xlsx
+++ b/CustomThailandScenarios/Data/Data Validation and Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mresb\Documents\Oxford\Small Group Exercise\MOD. Modelling\OSE. OSeMOSYS\ThailandEnergyModelling\CustomThailandScenarios\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3562A356-4B4B-49E0-91F8-A89DA277BDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CABF4FB-B609-44FD-8054-B641272C028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Energy Consumption" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
   <si>
     <t>Total</t>
   </si>
@@ -205,12 +205,6 @@
     <t>PWRCOA001</t>
   </si>
   <si>
-    <t>PWRCSP002</t>
-  </si>
-  <si>
-    <t>PWRDIST</t>
-  </si>
-  <si>
     <t>PWRHYD001</t>
   </si>
   <si>
@@ -223,15 +217,6 @@
     <t>PWRSOL001</t>
   </si>
   <si>
-    <t>PWRTRN</t>
-  </si>
-  <si>
-    <t>PWRTRNEXP</t>
-  </si>
-  <si>
-    <t>PWRTRNIMP</t>
-  </si>
-  <si>
     <t>PWRWND001</t>
   </si>
   <si>
@@ -244,9 +229,6 @@
     <t>GW</t>
   </si>
   <si>
-    <t>CSP</t>
-  </si>
-  <si>
     <t>Onshore wind</t>
   </si>
   <si>
@@ -274,16 +256,34 @@
     <t>YEAR 2021 Actual Thai Data</t>
   </si>
   <si>
-    <t>PWRBIO</t>
-  </si>
-  <si>
-    <t>PWRNGS</t>
-  </si>
-  <si>
-    <t>PWRHYD</t>
-  </si>
-  <si>
-    <t>PWROIL</t>
+    <t>https://www.global-climatescope.org/markets/th/</t>
+  </si>
+  <si>
+    <t>Geo</t>
+  </si>
+  <si>
+    <t>Small Hydro</t>
+  </si>
+  <si>
+    <t>Large Hydro</t>
+  </si>
+  <si>
+    <t>Biomass &amp; Waste</t>
+  </si>
+  <si>
+    <t>Model Values in FF_UpdatedCapacity</t>
+  </si>
+  <si>
+    <t>Biomass + Waste</t>
+  </si>
+  <si>
+    <t>Techno</t>
+  </si>
+  <si>
+    <t>ProductionByTechnologyAnnual</t>
+  </si>
+  <si>
+    <t>Output of the FF_UpdatedCapacity scenario</t>
   </si>
 </sst>
 </file>
@@ -395,6 +395,148 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>395027</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>79875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>672522</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>58796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A diagram of energy consumption&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7191DBD3-C3A1-8DF5-548B-6B1E6C704F29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7133083" y="3278394"/>
+          <a:ext cx="4863606" cy="2612995"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>471129</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>143387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>436627</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>149964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{089F70BA-6FCE-FB74-2C6E-D4A54AEB6CA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127500" y="4752258"/>
+          <a:ext cx="2239208" cy="4431093"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>264814</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>75139</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>204974</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>82639</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{520211FA-3918-B865-2FA3-57394274DB21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4094973" y="2977996"/>
+          <a:ext cx="2238255" cy="4724643"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1064,7 +1206,7 @@
   <dimension ref="B4:Z26"/>
   <sheetViews>
     <sheetView zoomScale="52" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,10 +1223,10 @@
         <v>33</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.35">
@@ -1533,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7319DC5-69BF-455D-B06E-60BC43ACC689}">
-  <dimension ref="A2:K17"/>
+  <dimension ref="A2:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D10"/>
+    <sheetView topLeftCell="D1" zoomScale="54" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,34 +1687,46 @@
     <col min="4" max="4" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K5" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I6" t="s">
         <v>18</v>
       </c>
@@ -1582,8 +1736,21 @@
       <c r="K6">
         <v>4.468</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="P6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6">
+        <v>7.468</v>
+      </c>
+      <c r="S6">
+        <f>100*R6/SUM(R$6:R$12)</f>
+        <v>15.47579575596817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I7" t="s">
         <v>7</v>
       </c>
@@ -1593,145 +1760,350 @@
       <c r="K7">
         <v>20.804200000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="P7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7">
+        <v>5.2590000000000003</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:S12" si="0">100*R7/SUM(R$6:R$12)</f>
+        <v>10.898126657824935</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>57</v>
       </c>
       <c r="K8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3.6389999999999998</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8">
+        <v>3.6389999999999998</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>7.5410311671087529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="J9" s="7" t="s">
         <v>58</v>
       </c>
       <c r="K9">
-        <v>42.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>0.30669761273209545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>59</v>
       </c>
       <c r="K10">
-        <v>3.6389999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>27.132000000000001</v>
+      </c>
+      <c r="P10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10">
+        <v>27.132000000000001</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>56.225132625994704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
       <c r="J11" s="7" t="s">
         <v>60</v>
       </c>
       <c r="K11">
-        <v>0.14799999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>3.0649999999999999</v>
+      </c>
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11">
+        <v>3.0649999999999999</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>6.3515417771883289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I12" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>61</v>
       </c>
       <c r="K12">
-        <v>27.132000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I13" t="s">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="P12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R12">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>3.201674403183024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K13" s="5">
+        <f>SUM(K6:K12)</f>
+        <v>60.801200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R14" s="5">
+        <f>SUM(R6:R12)</f>
+        <v>48.256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J21" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D28">
+        <f>100*C28/SUM(C$28:C$36)</f>
+        <v>5.8926130203177307E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29">
+        <v>0.19040000000000001</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D36" si="1">100*C29/SUM(C$28:C$36)</f>
+        <v>0.37398450635616537</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <v>2.9196999999999997</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>5.7348874118072253</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>1.524</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>2.9934474143214072</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13">
-        <v>3.0649999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14">
-        <v>42.88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15">
-        <v>0.13850000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16">
-        <v>4.4695</v>
-      </c>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.35">
-      <c r="I17" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17">
-        <v>1.5449999999999999</v>
+      <c r="C32">
+        <v>3.9369999999999998</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>7.733072486996968</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>2.96</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>5.814044846713494</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>4.6369999999999996</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>9.1080155250711048</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35">
+        <v>7.89</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>15.497572243435631</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>26.852799999999998</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>52.744386303995981</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C37" s="5">
+        <f>SUM(C28:C36)</f>
+        <v>50.911199999999994</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A042CCF-2282-4AE1-B0A0-1903225F5014}">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1739,17 +2111,25 @@
         <v>35176</v>
       </c>
       <c r="D6">
-        <f>100*C6/SUM(C$6:C$12)</f>
+        <f t="shared" ref="D6:D12" si="0">100*C6/SUM(C$6:C$12)</f>
         <v>19.914287493560238</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6">
-        <v>489.25330000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6">
+        <v>163.91659999999999</v>
+      </c>
+      <c r="M6">
+        <f>L6*278</f>
+        <v>45568.8148</v>
+      </c>
+      <c r="N6">
+        <f>100*M6/SUM(M$6:M$11)</f>
+        <v>25.803864835444216</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -1757,17 +2137,25 @@
         <v>657</v>
       </c>
       <c r="D7">
-        <f>100*C7/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>0.37194925185550026</v>
       </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7">
+        <v>123.6759</v>
+      </c>
+      <c r="M7">
+        <f>L7*278</f>
+        <v>34381.900199999996</v>
+      </c>
+      <c r="N7">
+        <f>100*M7/SUM(M$6:M$11)</f>
+        <v>19.469145937640938</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1775,17 +2163,25 @@
         <v>110052</v>
       </c>
       <c r="D8">
-        <f>100*C8/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>62.304047283411741</v>
       </c>
-      <c r="F8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <v>28.3385</v>
+      </c>
+      <c r="M8">
+        <f>L8*278</f>
+        <v>7878.1030000000001</v>
+      </c>
+      <c r="N8">
+        <f>100*M8/SUM(M$6:M$11)</f>
+        <v>4.4610663205510361</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1793,24 +2189,25 @@
         <v>4682</v>
       </c>
       <c r="D9">
-        <f>100*C9/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.6506337856734432</v>
       </c>
-      <c r="F9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9">
-        <f>SUM(I9:I10)</f>
-        <v>29.491099999999999</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9">
-        <v>28.3385</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9">
+        <v>1.1526000000000001</v>
+      </c>
+      <c r="M9">
+        <f>L9*278</f>
+        <v>320.4228</v>
+      </c>
+      <c r="N9">
+        <f>100*M9/SUM(M$6:M$11)</f>
+        <v>0.18144309123867258</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -1818,23 +2215,25 @@
         <v>17503</v>
       </c>
       <c r="D10">
-        <f>100*C10/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>9.9090224584883124</v>
       </c>
-      <c r="F10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10">
-        <v>98.069000000000003</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10">
-        <v>1.1526000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10">
+        <v>299.72980000000001</v>
+      </c>
+      <c r="M10">
+        <f>L10*278</f>
+        <v>83324.88440000001</v>
+      </c>
+      <c r="N10">
+        <f>100*M10/SUM(M$6:M$11)</f>
+        <v>47.183672955361011</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -1842,17 +2241,25 @@
         <v>5015</v>
       </c>
       <c r="D11">
-        <f>100*C11/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.8391560092166421</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11">
+      <c r="K11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11">
         <v>18.427099999999999</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <f>L11*278</f>
+        <v>5122.7338</v>
+      </c>
+      <c r="N11">
+        <f>100*M11/SUM(M$6:M$11)</f>
+        <v>2.9008068597641365</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1860,18 +2267,206 @@
         <v>3552</v>
       </c>
       <c r="D12">
-        <f>100*C12/SUM(C$6:C$12)</f>
+        <f t="shared" si="0"/>
         <v>2.01090371779412</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12">
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12">
         <v>7.7554999999999996</v>
+      </c>
+      <c r="M12">
+        <f>L12*278</f>
+        <v>2156.029</v>
+      </c>
+      <c r="N12">
+        <f>100*M12/SUM(M$6:M$11)</f>
+        <v>1.2208761878375198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="M13" s="5">
+        <f>SUM(M6:M12)</f>
+        <v>178752.88800000001</v>
+      </c>
+      <c r="N13">
+        <f>100*M13/SUM(M$6:M$11)</f>
+        <v>101.22087618783753</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>1.4</v>
+      </c>
+      <c r="D18">
+        <f>100*C18/SUM(C$18:C$26)</f>
+        <v>7.8577301823835302E-4</v>
+      </c>
+      <c r="E18">
+        <f>C18/278</f>
+        <v>5.0359712230215823E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <v>300.60000000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D26" si="1">100*C19/SUM(C$18:C$26)</f>
+        <v>0.1687166923446064</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E26" si="2">C19/278</f>
+        <v>1.081294964028777</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20">
+        <v>4239.3999999999996</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2.3794329525140525</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>15.249640287769783</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>4128.3999999999996</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2.3171323774965829</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>14.850359712230215</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>5052</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2.8355180629572567</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>18.172661870503596</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>716.4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0.40209127876139722</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>2.5769784172661869</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>36065</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>20.242074216261571</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>129.73021582733813</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25">
+        <v>14552.3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>8.1677176380785603</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>52.346402877697841</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26">
+        <v>113113</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>63.486531008567731</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>406.88129496402877</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="5">
+        <f>SUM(C18:C26)</f>
+        <v>178168.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2066,6 +2661,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D2C1BEFAF870748BACCC527472C8EB2" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487ae15c868a429603055564894ba096">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1041d1a3-2b21-46e0-8139-4e1099981477" xmlns:ns3="66da9736-248e-4959-a705-07c73b004417" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="194ea4c5e0e7bff924a75701159686b7" ns2:_="" ns3:_="">
     <xsd:import namespace="1041d1a3-2b21-46e0-8139-4e1099981477"/>
@@ -2242,22 +2852,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42A061F2-9FD0-4AE4-869A-5EC2633E6B02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="66da9736-248e-4959-a705-07c73b004417"/>
+    <ds:schemaRef ds:uri="1041d1a3-2b21-46e0-8139-4e1099981477"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415282BC-98EB-4742-A7DA-4D7B8E81DDAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3650B4B3-630C-4862-A6F7-7FA0C9B693D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2274,29 +2894,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{415282BC-98EB-4742-A7DA-4D7B8E81DDAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42A061F2-9FD0-4AE4-869A-5EC2633E6B02}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="66da9736-248e-4959-a705-07c73b004417"/>
-    <ds:schemaRef ds:uri="1041d1a3-2b21-46e0-8139-4e1099981477"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>